<commit_message>
pushing more e2e tests
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57901\macpro-onemac-automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5FDD3D-1B7F-4F05-AEDA-38BCA32D4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E64A35-8F87-46FA-AEA2-458722C02F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="1200" windowWidth="21600" windowHeight="11295" xr2:uid="{75A6ABCC-9875-48AC-9A16-7CDC4958549E}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{75A6ABCC-9875-48AC-9A16-7CDC4958549E}"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="53">
   <si>
     <t>PackageType</t>
   </si>
@@ -60,148 +60,130 @@
     <t>Medicaid SPA</t>
   </si>
   <si>
+    <t>MD-25-9261</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>MD-25-9266</t>
+  </si>
+  <si>
+    <t>Under Review</t>
+  </si>
+  <si>
+    <t>MD-25-9267</t>
+  </si>
+  <si>
+    <t>MD-25-9268</t>
+  </si>
+  <si>
+    <t>MD-25-9269</t>
+  </si>
+  <si>
+    <t>MD-25-9271</t>
+  </si>
+  <si>
+    <t>MD-25-9272</t>
+  </si>
+  <si>
+    <t>MD-25-9273</t>
+  </si>
+  <si>
+    <t>MD-25-9275</t>
+  </si>
+  <si>
+    <t>MD-25-9276</t>
+  </si>
+  <si>
+    <t>MD-25-9277</t>
+  </si>
+  <si>
+    <t>MD-25-9278</t>
+  </si>
+  <si>
+    <t>Disapproved</t>
+  </si>
+  <si>
+    <t>MD-25-9279</t>
+  </si>
+  <si>
+    <t>MD-25-9280</t>
+  </si>
+  <si>
+    <t>MD-2259.R00.00</t>
+  </si>
+  <si>
+    <t>1915(b)</t>
+  </si>
+  <si>
+    <t>Terminated</t>
+  </si>
+  <si>
+    <t>Waiver</t>
+  </si>
+  <si>
+    <t>MD-25-9282</t>
+  </si>
+  <si>
     <t>Submitted</t>
   </si>
   <si>
-    <t>MD-25-9231</t>
-  </si>
-  <si>
-    <t>MD-25-9232</t>
-  </si>
-  <si>
-    <t>MD-25-9233</t>
-  </si>
-  <si>
-    <t>MD-25-9234</t>
-  </si>
-  <si>
-    <t>MD-25-9235</t>
-  </si>
-  <si>
-    <t>MD-25-9236</t>
-  </si>
-  <si>
-    <t>MD-25-9237</t>
-  </si>
-  <si>
-    <t>MD-25-9238</t>
-  </si>
-  <si>
-    <t>MD-25-9239</t>
-  </si>
-  <si>
-    <t>MD-25-9240</t>
-  </si>
-  <si>
-    <t>CHIP SPA</t>
-  </si>
-  <si>
-    <t>MD-25-9241</t>
-  </si>
-  <si>
-    <t>MD-25-9242</t>
-  </si>
-  <si>
-    <t>MD-25-9243</t>
-  </si>
-  <si>
-    <t>MD-25-9244</t>
-  </si>
-  <si>
-    <t>MD-25-9245</t>
-  </si>
-  <si>
-    <t>Waiver</t>
-  </si>
-  <si>
-    <t>1915(b)</t>
+    <t>Pending-Concurrence</t>
+  </si>
+  <si>
+    <t>MD-25-9283</t>
+  </si>
+  <si>
+    <t>MD-25-9284</t>
+  </si>
+  <si>
+    <t>MD-25-9285</t>
+  </si>
+  <si>
+    <t>MD-25-9286</t>
+  </si>
+  <si>
+    <t>MD-25-9287</t>
+  </si>
+  <si>
+    <t>Pending-Approval</t>
+  </si>
+  <si>
+    <t>MD-25-9288</t>
   </si>
   <si>
     <t>Initial</t>
   </si>
   <si>
-    <t>MD-2242.R00.00</t>
-  </si>
-  <si>
-    <t>1915(c)</t>
-  </si>
-  <si>
-    <t>MD-2243.R00.00</t>
-  </si>
-  <si>
-    <t>MD-2244.R00.00</t>
-  </si>
-  <si>
-    <t>MD-2245.R00.00</t>
-  </si>
-  <si>
-    <t>MD-2246.R00.00</t>
-  </si>
-  <si>
-    <t>MD-2247.R00.00</t>
-  </si>
-  <si>
-    <t>Package Withdrawn</t>
-  </si>
-  <si>
-    <t>MD-25-9246</t>
-  </si>
-  <si>
-    <t>MD-25-9247</t>
-  </si>
-  <si>
-    <t>MD-25-9248</t>
-  </si>
-  <si>
-    <t>MD-25-9249</t>
-  </si>
-  <si>
-    <t>MD-25-9250</t>
-  </si>
-  <si>
-    <t>MD-25-9251</t>
-  </si>
-  <si>
-    <t>MD-25-9252</t>
-  </si>
-  <si>
-    <t>MD-25-9253</t>
-  </si>
-  <si>
-    <t>MD-25-9254</t>
-  </si>
-  <si>
-    <t>MD-25-9255</t>
-  </si>
-  <si>
-    <t>MD-25-9256</t>
-  </si>
-  <si>
-    <t>MD-25-9257</t>
-  </si>
-  <si>
-    <t>MD-25-9258</t>
-  </si>
-  <si>
-    <t>MD-25-9259</t>
-  </si>
-  <si>
-    <t>MD-25-9260</t>
-  </si>
-  <si>
-    <t>MD-25-9261</t>
-  </si>
-  <si>
-    <t>MD-25-9262</t>
-  </si>
-  <si>
-    <t>MD-25-9263</t>
-  </si>
-  <si>
-    <t>MD-25-9264</t>
-  </si>
-  <si>
-    <t>MD-25-9265</t>
+    <t>MD-2260.R00.00</t>
+  </si>
+  <si>
+    <t>MD-25-9289</t>
+  </si>
+  <si>
+    <t>MD-25-9290</t>
+  </si>
+  <si>
+    <t>MD-25-9291</t>
+  </si>
+  <si>
+    <t>MD-25-9292</t>
+  </si>
+  <si>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>MD-25-9293</t>
+  </si>
+  <si>
+    <t>MD-25-9294</t>
+  </si>
+  <si>
+    <t>MD-25-9295</t>
+  </si>
+  <si>
+    <t>MD-25-9296</t>
   </si>
 </sst>
 </file>
@@ -246,10 +228,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5CF9F-A3EF-4F4C-99C9-E52FA1956C25}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +583,7 @@
     <col min="3" max="3" customWidth="true" width="13.5703125"/>
     <col min="4" max="4" customWidth="true" width="27.140625"/>
     <col min="5" max="5" customWidth="true" width="20.7109375"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125"/>
+    <col min="6" max="6" customWidth="true" width="26.42578125"/>
     <col min="7" max="7" customWidth="true" width="30.28515625"/>
   </cols>
   <sheetData>
@@ -639,10 +624,10 @@
         <v>9</v>
       </c>
       <c r="E2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>11</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>9</v>
@@ -665,7 +650,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>9</v>
@@ -685,10 +670,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>11</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>9</v>
@@ -708,10 +693,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>9</v>
@@ -731,10 +716,10 @@
         <v>9</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>9</v>
@@ -754,10 +739,10 @@
         <v>9</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>9</v>
@@ -777,10 +762,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>9</v>
@@ -800,10 +785,10 @@
         <v>9</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>9</v>
@@ -823,10 +808,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>9</v>
@@ -846,10 +831,10 @@
         <v>9</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>9</v>
@@ -863,7 +848,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s" s="0">
         <v>9</v>
@@ -872,7 +857,7 @@
         <v>23</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s" s="0">
         <v>9</v>
@@ -895,7 +880,7 @@
         <v>24</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s" s="0">
         <v>9</v>
@@ -909,16 +894,16 @@
         <v>8</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E14" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s" s="0">
         <v>25</v>
-      </c>
-      <c r="F14" t="s" s="0">
-        <v>9</v>
       </c>
       <c r="G14" t="s" s="0">
         <v>9</v>
@@ -938,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s" s="0">
         <v>9</v>
@@ -949,160 +934,160 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s" s="0">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s" s="0">
         <v>9</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s" s="0">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G17" t="s" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s" s="0">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" t="s" s="0">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="F19" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E20" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="F20" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="G20" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="F21" t="s" s="0">
-        <v>9</v>
-      </c>
       <c r="G21" t="s" s="0">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" t="s" s="0">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s" s="0">
         <v>9</v>
@@ -1122,10 +1107,10 @@
         <v>9</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G23" t="s" s="0">
         <v>9</v>
@@ -1133,22 +1118,22 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>8</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s" s="0">
         <v>9</v>
@@ -1168,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G25" t="s" s="0">
         <v>9</v>
@@ -1191,10 +1176,10 @@
         <v>9</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s" s="0">
         <v>9</v>
@@ -1214,10 +1199,10 @@
         <v>9</v>
       </c>
       <c r="E27" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s" s="0">
         <v>9</v>
@@ -1237,10 +1222,10 @@
         <v>9</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G28" t="s" s="0">
         <v>9</v>
@@ -1260,10 +1245,10 @@
         <v>9</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s" s="0">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G29" t="s" s="0">
         <v>9</v>
@@ -1283,10 +1268,10 @@
         <v>9</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s" s="0">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s" s="0">
         <v>9</v>
@@ -1306,10 +1291,10 @@
         <v>9</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s" s="0">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s" s="0">
         <v>9</v>
@@ -1329,242 +1314,12 @@
         <v>9</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B33" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E33" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="F33" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G33" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C34" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E34" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F34" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G34" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C35" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E35" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="F35" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G35" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B36" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C36" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="F36" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G36" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B37" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C37" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E37" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="F37" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G37" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B38" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C38" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E38" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="F38" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G38" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C39" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E39" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="F39" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G39" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C40" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="F40" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G40" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C41" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E41" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="F41" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G41" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B42" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C42" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E42" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="F42" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="G42" t="s" s="0">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Update Excel counters (state_counters + packages)
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="180">
   <si>
     <t>PackageType</t>
   </si>
@@ -529,6 +529,42 @@
   </si>
   <si>
     <t>MD-25-9422</t>
+  </si>
+  <si>
+    <t>MD-25-9423</t>
+  </si>
+  <si>
+    <t>MD-25-9424</t>
+  </si>
+  <si>
+    <t>MD-25-9425</t>
+  </si>
+  <si>
+    <t>MD-25-9426</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.34</t>
+  </si>
+  <si>
+    <t>MD-25-9427</t>
+  </si>
+  <si>
+    <t>MD-25-9428</t>
+  </si>
+  <si>
+    <t>MD-25-9429</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.35</t>
+  </si>
+  <si>
+    <t>MD-25-9430</t>
+  </si>
+  <si>
+    <t>MD-2275.R00.00</t>
+  </si>
+  <si>
+    <t>MD-25-9431</t>
   </si>
 </sst>
 </file>
@@ -915,7 +951,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5CF9F-A3EF-4F4C-99C9-E52FA1956C25}">
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
       <selection activeCell="F125" sqref="F125"/>
@@ -4244,6 +4280,282 @@
         <v>9</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B145" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C145" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D145" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E145" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="F145" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G145" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B146" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C146" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D146" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E146" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="F146" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G146" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B147" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C147" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D147" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E147" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="F147" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G147" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B148" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C148" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D148" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E148" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="F148" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G148" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B149" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C149" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D149" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="E149" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="F149" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G149" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B150" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C150" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D150" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E150" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="F150" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G150" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B151" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C151" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D151" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E151" t="s" s="0">
+        <v>174</v>
+      </c>
+      <c r="F151" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G151" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B152" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C152" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D152" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E152" t="s" s="0">
+        <v>175</v>
+      </c>
+      <c r="F152" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G152" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B153" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C153" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D153" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="E153" t="s" s="0">
+        <v>176</v>
+      </c>
+      <c r="F153" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="G153" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B154" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C154" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D154" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E154" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="F154" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G154" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B155" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C155" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D155" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E155" t="s" s="0">
+        <v>178</v>
+      </c>
+      <c r="F155" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G155" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B156" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C156" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D156" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E156" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="F156" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G156" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding ChipSPA OneMAC script
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="191">
   <si>
     <t>PackageType</t>
   </si>
@@ -589,6 +589,15 @@
   </si>
   <si>
     <t>MD-25-9438</t>
+  </si>
+  <si>
+    <t>CHIP SPA</t>
+  </si>
+  <si>
+    <t>MD-25-9439</t>
+  </si>
+  <si>
+    <t>MD-25-9440</t>
   </si>
 </sst>
 </file>
@@ -975,7 +984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5CF9F-A3EF-4F4C-99C9-E52FA1956C25}">
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
       <selection activeCell="F125" sqref="F125"/>
@@ -4764,6 +4773,52 @@
         <v>9</v>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B165" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C165" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="D165" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E165" t="s" s="0">
+        <v>189</v>
+      </c>
+      <c r="F165" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G165" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B166" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C166" t="s" s="0">
+        <v>188</v>
+      </c>
+      <c r="D166" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E166" t="s" s="0">
+        <v>190</v>
+      </c>
+      <c r="F166" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G166" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing waiver termination flow
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="73">
   <si>
     <t>PackageType</t>
   </si>
@@ -166,6 +166,84 @@
   </si>
   <si>
     <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.55</t>
+  </si>
+  <si>
+    <t>MD-25-9518</t>
+  </si>
+  <si>
+    <t>MD-25-9519</t>
+  </si>
+  <si>
+    <t>MD-25-9520</t>
+  </si>
+  <si>
+    <t>MD-25-9521</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.56</t>
+  </si>
+  <si>
+    <t>MD-25-9522</t>
+  </si>
+  <si>
+    <t>MD-25-9523</t>
+  </si>
+  <si>
+    <t>MD-25-9524</t>
+  </si>
+  <si>
+    <t>MD-25-9525</t>
+  </si>
+  <si>
+    <t>MD-25-9526</t>
+  </si>
+  <si>
+    <t>MD-25-9527</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.57</t>
+  </si>
+  <si>
+    <t>MD-25-9528</t>
+  </si>
+  <si>
+    <t>MD-2281.R00.00</t>
+  </si>
+  <si>
+    <t>MD-25-9529</t>
+  </si>
+  <si>
+    <t>MD-25-9530</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.58</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.59</t>
+  </si>
+  <si>
+    <t>Pending-Approval</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.60</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.61</t>
+  </si>
+  <si>
+    <t>Unsubmitted</t>
+  </si>
+  <si>
+    <t>MD-2282.R00.00</t>
+  </si>
+  <si>
+    <t>Terminated</t>
+  </si>
+  <si>
+    <t>MD-2283.R00.00</t>
   </si>
 </sst>
 </file>
@@ -549,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5CF9F-A3EF-4F4C-99C9-E52FA1956C25}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -1069,6 +1147,535 @@
         <v>8</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G32" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F33" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G33" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="F34" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F35" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="F36" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G36" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="F37" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G37" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="F38" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G38" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="F39" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F41" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G41" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G42" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="F43" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="G43" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="F44" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G44" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="F45" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="G45" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated excel data sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="125">
   <si>
     <t>PackageType</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>MD-25-9564</t>
+  </si>
+  <si>
+    <t>MD-25-9565</t>
+  </si>
+  <si>
+    <t>MD-25-9566</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.73</t>
+  </si>
+  <si>
+    <t>MD-2260.R00.74</t>
   </si>
 </sst>
 </file>
@@ -771,7 +783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5CF9F-A3EF-4F4C-99C9-E52FA1956C25}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -2924,6 +2936,98 @@
         <v>8</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B94" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D94" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E94" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="F94" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G94" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B95" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D95" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E95" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="F95" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G95" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B96" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D96" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="F96" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G96" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B97" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D97" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E97" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="F97" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G97" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testing write back and commit
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57901\macpro-onemac-automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1653B8A7-EF82-49D0-B78D-A01E2682FDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACA6FAF-03A0-4A38-BE36-2726B7B514BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34935" yWindow="1680" windowWidth="21600" windowHeight="11295" xr2:uid="{75A6ABCC-9875-48AC-9A16-7CDC4958549E}"/>
   </bookViews>
@@ -399,7 +399,7 @@
     <t>MD-2260.R00.73</t>
   </si>
   <si>
-    <t>MD-2260.R00.78</t>
+    <t>MD-2260.R00.79</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
CI: Update Excel source-of-truth
</commit_message>
<xml_diff>
--- a/src/test/resources/packages.xlsx
+++ b/src/test/resources/packages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="127">
   <si>
     <t>PackageType</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>MD-2260.R00.80</t>
+  </si>
+  <si>
+    <t>MD-25-9567</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A5CF9F-A3EF-4F4C-99C9-E52FA1956C25}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
       <selection activeCell="E97" sqref="E97"/>
@@ -3054,6 +3057,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B99" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D99" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E99" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="F99" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G99" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>